<commit_message>
update unget none edoc
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.Report/eFMS.API.Report/FormatExcel/TemplateExport/Template-Report-eDOC.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.Report/eFMS.API.Report/FormatExcel/TemplateExport/Template-Report-eDOC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="28785" windowHeight="4875"/>
+    <workbookView xWindow="0" yWindow="2250" windowWidth="28785" windowHeight="4875"/>
   </bookViews>
   <sheets>
     <sheet name="EDoc Report" sheetId="2" r:id="rId1"/>
@@ -30,9 +30,6 @@
 Website: www.itlvn.com</t>
   </si>
   <si>
-    <t>JOB COSTING SUMMARY REPORT</t>
-  </si>
-  <si>
     <t>Job No.</t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>{UserExport}</t>
+  </si>
+  <si>
+    <t>JOB FILE eDOC ATTACHMENT SUMMARY REPORT</t>
   </si>
 </sst>
 </file>
@@ -263,27 +263,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,7 +607,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -640,8 +640,8 @@
       <c r="I2" s="8"/>
     </row>
     <row r="4" spans="1:16" ht="17.25">
-      <c r="A4" s="9" t="s">
-        <v>2</v>
+      <c r="A4" s="15" t="s">
+        <v>36</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -655,8 +655,8 @@
       <c r="K4" s="10"/>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="11" t="s">
-        <v>34</v>
+      <c r="A5" s="16" t="s">
+        <v>33</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -686,126 +686,126 @@
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="N7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="L7" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="M7" s="14" t="s">
+      <c r="O7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="N7" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="O7" s="14" t="s">
+      <c r="P7" s="11" t="s">
         <v>14</v>
-      </c>
-      <c r="P7" s="14" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="I9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="K9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="L9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="M9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="N9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="O9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="P9" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="13" t="s">
-        <v>36</v>
+      <c r="A10" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -820,6 +820,14 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
     <mergeCell ref="A10:K10"/>
     <mergeCell ref="P7:P8"/>
     <mergeCell ref="L7:L8"/>
@@ -831,14 +839,6 @@
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="H7:H8"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>